<commit_message>
Recurso 110  tema 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC140.xlsx
+++ b/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC140.xlsx
@@ -719,7 +719,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -763,12 +763,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1291,7 +1285,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1467,6 +1461,26 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1551,42 +1565,6 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2493,9 +2471,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2533,14 +2511,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="F2" s="67" t="s">
+      <c r="D2" s="83"/>
+      <c r="F2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="68"/>
+      <c r="G2" s="76"/>
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
       <c r="J2" s="16"/>
@@ -2550,12 +2528,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="84">
         <v>11</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="D3" s="85"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="78"/>
       <c r="H3" s="42"/>
       <c r="I3" s="42"/>
       <c r="J3" s="16"/>
@@ -2565,10 +2543,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="5"/>
       <c r="F4" s="41" t="s">
         <v>55</v>
@@ -2586,10 +2564,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="87"/>
       <c r="E5" s="5"/>
       <c r="F5" s="39" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2640,12 +2618,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2690,242 +2668,242 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="106" t="str">
+      <c r="C10" s="69" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="107" t="s">
+      <c r="E10" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="107" t="str">
+      <c r="F10" s="70" t="str">
         <f t="shared" ref="F10" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC140_IMG01n.jpg</v>
       </c>
-      <c r="G10" s="107" t="str">
+      <c r="G10" s="70" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H10" s="107" t="str">
+      <c r="H10" s="70" t="str">
         <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC140_IMG01a.jpg</v>
       </c>
-      <c r="I10" s="107" t="s">
+      <c r="I10" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J10" s="108" t="s">
+      <c r="J10" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="K10" s="109" t="s">
+      <c r="K10" s="72" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="100" t="str">
-        <f t="shared" ref="C11:C19" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+      <c r="C11" s="69" t="str">
+        <f t="shared" ref="C11:C15" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="101" t="str">
-        <f t="shared" ref="F11:F19" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+      <c r="F11" s="70" t="str">
+        <f t="shared" ref="F11:F15" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC140_IMG02n.jpg</v>
       </c>
-      <c r="G11" s="101" t="str">
+      <c r="G11" s="70" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H11" s="101" t="str">
-        <f t="shared" ref="H11:H19" si="3">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+      <c r="H11" s="70" t="str">
+        <f t="shared" ref="H11:H15" si="3">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC140_IMG02a.jpg</v>
       </c>
-      <c r="I11" s="101" t="s">
+      <c r="I11" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="102" t="s">
+      <c r="J11" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="K11" s="103" t="s">
+      <c r="K11" s="72" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="106" t="str">
+      <c r="C12" s="69" t="str">
         <f t="shared" si="1"/>
         <v>Recurso F13</v>
       </c>
-      <c r="D12" s="107" t="s">
+      <c r="D12" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="107" t="s">
+      <c r="E12" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="107" t="str">
+      <c r="F12" s="70" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC140_IMG03n.jpg</v>
       </c>
-      <c r="G12" s="107" t="str">
+      <c r="G12" s="70" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H12" s="107" t="str">
+      <c r="H12" s="70" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC140_IMG03a.jpg</v>
       </c>
-      <c r="I12" s="107" t="s">
+      <c r="I12" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J12" s="108" t="s">
+      <c r="J12" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="K12" s="109" t="s">
+      <c r="K12" s="72" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="106" t="str">
+      <c r="C13" s="69" t="str">
         <f t="shared" si="1"/>
         <v>Recurso F13</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="107" t="s">
+      <c r="E13" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="107" t="str">
+      <c r="F13" s="70" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC140_IMG04n.jpg</v>
       </c>
-      <c r="G13" s="107" t="str">
+      <c r="G13" s="70" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H13" s="107" t="str">
+      <c r="H13" s="70" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC140_IMG04a.jpg</v>
       </c>
-      <c r="I13" s="107" t="s">
+      <c r="I13" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J13" s="108" t="s">
+      <c r="J13" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="K13" s="109" t="s">
+      <c r="K13" s="72" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="106" t="str">
+      <c r="C14" s="69" t="str">
         <f t="shared" si="1"/>
         <v>Recurso F13</v>
       </c>
-      <c r="D14" s="107" t="s">
+      <c r="D14" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="107" t="s">
+      <c r="E14" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="107" t="str">
+      <c r="F14" s="70" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC140_IMG05n.jpg</v>
       </c>
-      <c r="G14" s="107" t="str">
+      <c r="G14" s="70" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H14" s="107" t="str">
+      <c r="H14" s="70" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC140_IMG05a.jpg</v>
       </c>
-      <c r="I14" s="107" t="s">
+      <c r="I14" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J14" s="108" t="s">
+      <c r="J14" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="K14" s="109" t="s">
+      <c r="K14" s="72" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="106" t="str">
+      <c r="C15" s="69" t="str">
         <f t="shared" si="1"/>
         <v>Recurso F13</v>
       </c>
-      <c r="D15" s="107" t="s">
+      <c r="D15" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="107" t="s">
+      <c r="E15" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="107" t="str">
+      <c r="F15" s="70" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC140_IMG06n.jpg</v>
       </c>
-      <c r="G15" s="107" t="str">
+      <c r="G15" s="70" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="H15" s="107" t="str">
+      <c r="H15" s="70" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC140_IMG06a.jpg</v>
       </c>
-      <c r="I15" s="107" t="s">
+      <c r="I15" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="J15" s="108" t="s">
+      <c r="J15" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="K15" s="109" t="s">
+      <c r="K15" s="72" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="110"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="22"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -2934,11 +2912,11 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="111"/>
+      <c r="K16" s="74"/>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="110"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="22"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -2951,7 +2929,7 @@
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="110"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="22"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -2964,7 +2942,7 @@
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="110"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="22"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -2977,7 +2955,7 @@
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="110"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="22"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -3824,25 +3802,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="33"/>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95"/>
       <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -3850,11 +3828,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="34"/>
       <c r="H3" s="24" t="s">
         <v>18</v>
@@ -3905,11 +3883,11 @@
       <c r="C5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="94" t="str">
+      <c r="D5" s="102" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_02_CO</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="103"/>
       <c r="F5" s="34"/>
       <c r="H5" s="24" t="s">
         <v>22</v>
@@ -3954,12 +3932,12 @@
       <c r="C7" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="80" t="str">
+      <c r="D7" s="88" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_CO.xls</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
       <c r="H7" s="24" t="s">
         <v>24</v>
       </c>
@@ -4053,14 +4031,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="84"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92"/>
       <c r="I13" s="24" t="s">
         <v>33</v>
       </c>
@@ -4093,12 +4071,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="33"/>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="87"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="J15" s="24">
         <v>12</v>
       </c>
@@ -4138,12 +4116,12 @@
       <c r="C17" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="88" t="str">
+      <c r="D17" s="96" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_02_REC130</v>
       </c>
-      <c r="E17" s="89"/>
-      <c r="F17" s="90"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
       <c r="J17" s="24">
         <v>14</v>
       </c>
@@ -4159,12 +4137,12 @@
       <c r="C18" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="80" t="str">
+      <c r="D18" s="88" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_REC130.xls</v>
       </c>
-      <c r="E18" s="80"/>
-      <c r="F18" s="81"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="89"/>
       <c r="J18" s="24">
         <v>15</v>
       </c>
@@ -4556,41 +4534,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
+      <c r="A2" s="104"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
       <c r="H2" s="43" t="s">
         <v>65</v>
       </c>

</xml_diff>